<commit_message>
added some more pre-processing
</commit_message>
<xml_diff>
--- a/results_firstround_models.xlsx
+++ b/results_firstround_models.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855"/>
   </bookViews>
   <sheets>
-    <sheet name="results" sheetId="2" r:id="rId1"/>
+    <sheet name="results_allgenres" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -437,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,4 +791,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tried more anti-overfitting methods in random forest
</commit_message>
<xml_diff>
--- a/results_firstround_models.xlsx
+++ b/results_firstround_models.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JupData\country_music\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3855"/>
   </bookViews>
   <sheets>
     <sheet name="results_allgenres" sheetId="2" r:id="rId1"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
+    <sheet name="results_tfidf" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>x_train</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>x_train_stop</t>
+  </si>
+  <si>
+    <t>x_train_pca (10 components, 28% explained var)</t>
   </si>
 </sst>
 </file>
@@ -438,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,12 +798,171 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.42</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.39</v>
+      </c>
+      <c r="H4">
+        <v>0.12</v>
+      </c>
+      <c r="I4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.43</v>
+      </c>
+      <c r="D5">
+        <v>0.09</v>
+      </c>
+      <c r="E5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.42</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.42</v>
+      </c>
+      <c r="D6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.44</v>
+      </c>
+      <c r="F6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.32</v>
+      </c>
+      <c r="H6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>